<commit_message>
Updated to use late january bvc sheet Fixed first bvc store not being loaded correctly
</commit_message>
<xml_diff>
--- a/caches/beer-names.xlsx
+++ b/caches/beer-names.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="128">
   <si>
     <t xml:space="preserve">SAFE SPACE</t>
   </si>
@@ -401,6 +401,9 @@
   </si>
   <si>
     <t xml:space="preserve">Imperial Stout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Appl Crisp</t>
   </si>
 </sst>
 </file>
@@ -517,10 +520,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C85"/>
+  <dimension ref="A1:C86"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A29" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A68" activeCellId="0" sqref="A68:C85"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A47" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A89" activeCellId="0" sqref="89:89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1463,6 +1466,17 @@
         <v>4</v>
       </c>
     </row>
+    <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C86" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Updated map March 2024
</commit_message>
<xml_diff>
--- a/caches/beer-names.xlsx
+++ b/caches/beer-names.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="132">
   <si>
     <t xml:space="preserve">SAFE SPACE</t>
   </si>
@@ -404,6 +404,18 @@
   </si>
   <si>
     <t xml:space="preserve">Appl Crisp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WHITE MOUNTAIN WHITE ALE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">White Mountain Ale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQUIRREL FIGHTS NUT BROWN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OKTOBERFEST MARZEN</t>
   </si>
 </sst>
 </file>
@@ -520,14 +532,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C86"/>
+  <dimension ref="A1:C89"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A47" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A89" activeCellId="0" sqref="89:89"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A44" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D75" activeCellId="0" sqref="D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.71"/>
   </cols>
   <sheetData>
@@ -1474,6 +1487,39 @@
         <v>107</v>
       </c>
       <c r="C86" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C87" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C88" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C89" s="0" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>